<commit_message>
Added meeting + other files
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - University of Pretoria\Desktop\Computer Science\Year 2\Semester 2\COS 214 (Software modelling)\Prac\COS-214-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E219F259-D5EE-44AE-BCD3-4AFF43AC6E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16AD618-03A3-4D6D-BE1E-0B8E7D1DA3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1965" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Monday</t>
   </si>
@@ -66,22 +66,13 @@
     <t>IMY 220 EO</t>
   </si>
   <si>
-    <t>IMY 220 A7</t>
-  </si>
-  <si>
     <t>COS 226 A2</t>
   </si>
   <si>
     <t>COS 214 EO3</t>
   </si>
   <si>
-    <t>IMY 220 A8</t>
-  </si>
-  <si>
     <t>COS 284 CT</t>
-  </si>
-  <si>
-    <t>IMY 220 A9</t>
   </si>
   <si>
     <t>IMY 220 Project</t>
@@ -278,9 +269,6 @@
     <t>Meeting</t>
   </si>
   <si>
-    <t>Finishing touches</t>
-  </si>
-  <si>
     <t>Finilize UML</t>
   </si>
   <si>
@@ -300,6 +288,18 @@
   </si>
   <si>
     <t>Done*</t>
+  </si>
+  <si>
+    <t>Finishing touches*</t>
+  </si>
+  <si>
+    <t>Feedback*</t>
+  </si>
+  <si>
+    <t>Busy</t>
+  </si>
+  <si>
+    <t>No there yet</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +379,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -530,11 +548,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -563,6 +578,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,482 +869,488 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="2" max="8" width="18.140625" customWidth="1"/>
     <col min="10" max="16" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="18">
+      <c r="B3" s="17"/>
+      <c r="C3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="15">
         <v>3</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="15">
         <v>4</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="15">
         <v>5</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+      <c r="B5" s="15">
         <v>7</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="15">
         <v>8</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>9</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>10</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <v>11</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="13">
         <v>12</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="13">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>14</v>
+      </c>
+      <c r="C7" s="15">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13">
+        <v>16</v>
+      </c>
+      <c r="E7" s="15">
+        <v>17</v>
+      </c>
+      <c r="F7" s="13">
+        <v>18</v>
+      </c>
+      <c r="G7" s="13">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13">
+        <v>23</v>
+      </c>
+      <c r="E9" s="15">
+        <v>24</v>
+      </c>
+      <c r="F9" s="9">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15">
+        <v>26</v>
+      </c>
+      <c r="H9" s="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13">
+        <v>28</v>
+      </c>
+      <c r="C11" s="15">
+        <v>29</v>
+      </c>
+      <c r="D11" s="13">
+        <v>30</v>
+      </c>
+      <c r="E11" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="14" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="13">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
+        <v>4</v>
+      </c>
+      <c r="C18" s="13">
+        <v>5</v>
+      </c>
+      <c r="D18" s="13">
+        <v>6</v>
+      </c>
+      <c r="E18" s="15">
+        <v>7</v>
+      </c>
+      <c r="F18" s="15">
+        <v>8</v>
+      </c>
+      <c r="G18" s="15">
+        <v>9</v>
+      </c>
+      <c r="H18" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <v>11</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="C20" s="15">
         <v>12</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="D20" s="15">
+        <v>13</v>
+      </c>
+      <c r="E20" s="15">
+        <v>14</v>
+      </c>
+      <c r="F20" s="15">
+        <v>15</v>
+      </c>
+      <c r="G20" s="15">
+        <v>16</v>
+      </c>
+      <c r="H20" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
+        <v>18</v>
+      </c>
+      <c r="C22" s="15">
+        <v>19</v>
+      </c>
+      <c r="D22" s="15">
+        <v>20</v>
+      </c>
+      <c r="E22" s="15">
+        <v>21</v>
+      </c>
+      <c r="F22" s="15">
+        <v>22</v>
+      </c>
+      <c r="G22" s="15">
+        <v>23</v>
+      </c>
+      <c r="H22" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15">
+        <v>26</v>
+      </c>
+      <c r="D24" s="15">
+        <v>27</v>
+      </c>
+      <c r="E24" s="15">
         <v>28</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="F24" s="15">
+        <v>29</v>
+      </c>
+      <c r="G24" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="27" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
-        <v>14</v>
-      </c>
-      <c r="C7" s="16">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8">
-        <v>16</v>
-      </c>
-      <c r="E7" s="16">
-        <v>17</v>
-      </c>
-      <c r="F7" s="16">
-        <v>18</v>
-      </c>
-      <c r="G7" s="16">
-        <v>19</v>
-      </c>
-      <c r="H7" s="10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
-        <v>21</v>
-      </c>
-      <c r="C9" s="16">
+    <row r="31" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="8">
+      <c r="J31" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="18">
+      <c r="J32" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="12">
-        <v>25</v>
-      </c>
-      <c r="G9" s="18">
-        <v>26</v>
-      </c>
-      <c r="H9" s="16">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
-        <v>28</v>
-      </c>
-      <c r="C11" s="16">
-        <v>29</v>
-      </c>
-      <c r="D11" s="8">
-        <v>30</v>
-      </c>
-      <c r="E11" s="18">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="14" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="18">
-        <v>2</v>
-      </c>
-      <c r="H16" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
-        <v>4</v>
-      </c>
-      <c r="C18" s="16">
-        <v>5</v>
-      </c>
-      <c r="D18" s="16">
-        <v>6</v>
-      </c>
-      <c r="E18" s="18">
-        <v>7</v>
-      </c>
-      <c r="F18" s="18">
-        <v>8</v>
-      </c>
-      <c r="G18" s="18">
-        <v>9</v>
-      </c>
-      <c r="H18" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
-        <v>11</v>
-      </c>
-      <c r="C20" s="18">
-        <v>12</v>
-      </c>
-      <c r="D20" s="18">
-        <v>13</v>
-      </c>
-      <c r="E20" s="18">
-        <v>14</v>
-      </c>
-      <c r="F20" s="18">
-        <v>15</v>
-      </c>
-      <c r="G20" s="18">
-        <v>16</v>
-      </c>
-      <c r="H20" s="18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="18">
-        <v>18</v>
-      </c>
-      <c r="C22" s="18">
-        <v>19</v>
-      </c>
-      <c r="D22" s="18">
-        <v>20</v>
-      </c>
-      <c r="E22" s="18">
-        <v>21</v>
-      </c>
-      <c r="F22" s="18">
-        <v>22</v>
-      </c>
-      <c r="G22" s="18">
-        <v>23</v>
-      </c>
-      <c r="H22" s="18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="18">
-        <v>25</v>
-      </c>
-      <c r="C24" s="18">
-        <v>26</v>
-      </c>
-      <c r="D24" s="18">
-        <v>27</v>
-      </c>
-      <c r="E24" s="18">
-        <v>28</v>
-      </c>
-      <c r="F24" s="18">
-        <v>29</v>
-      </c>
-      <c r="G24" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="27" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="1" t="s">
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="29" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1333,6 +1359,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>